<commit_message>
Bug fix for DefectStatus test
</commit_message>
<xml_diff>
--- a/Project_RTM.xlsx
+++ b/Project_RTM.xlsx
@@ -91,7 +91,7 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Successful Login</t>
+    <t>Login with valid credentials</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to log in successfully. </t>
@@ -103,16 +103,16 @@
     <t>FAILED</t>
   </si>
   <si>
-    <t>Wrong Password</t>
+    <t>Login with wrong username and correct password</t>
+  </si>
+  <si>
+    <t>Incorrect username should result in corresponding alert, and failed login.</t>
+  </si>
+  <si>
+    <t>Login with correct username and wrong password</t>
   </si>
   <si>
     <t>Incorrect password should result in corresponding alert, and failed login.</t>
-  </si>
-  <si>
-    <t>Wrong Username</t>
-  </si>
-  <si>
-    <t>Incorrect username should result in corresponding alert, and failed login.</t>
   </si>
   <si>
     <t>Navigation</t>
@@ -268,12 +268,12 @@
     <font>
       <b val="1"/>
       <sz val="24"/>
-      <color indexed="13"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="13"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -304,7 +304,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -361,11 +361,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -374,7 +374,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -382,17 +382,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -409,7 +409,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -417,12 +417,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -431,28 +442,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -463,7 +463,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -473,28 +473,28 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,24 +518,24 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,28 +544,28 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,28 +597,28 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -636,20 +636,20 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -780,8 +780,8 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffe7e6e6"/>
       <rgbColor rgb="ffcfcfcf"/>
       <rgbColor rgb="ffd9dce1"/>
@@ -1856,7 +1856,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1974,16 +1974,19 @@
       <c r="D12" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13">
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="7"/>
       <c r="B13" t="s" s="3">
         <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
@@ -1991,6 +1994,7 @@
       <c r="D14" t="s" s="5">
         <v>8</v>
       </c>
+      <c r="E14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2000,7 +2004,8 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Sheet1'!R1C1" tooltip="" display="Sheet1"/>
-    <hyperlink ref="D12" location="'STATUS'!R1C1" tooltip="" display="STATUS"/>
+    <hyperlink ref="D12" location="'Sheet1'!R1C1" tooltip="" display="Sheet1"/>
+    <hyperlink ref="D14" location="'STATUS'!R1C1" tooltip="" display="STATUS"/>
     <hyperlink ref="D12" location="'Sheet1'!R1C1" tooltip="" display="Sheet1"/>
     <hyperlink ref="D14" location="'STATUS'!R1C1" tooltip="" display="STATUS"/>
   </hyperlinks>
@@ -2023,7 +2028,7 @@
     <col min="1" max="1" width="34.1719" style="25" customWidth="1"/>
     <col min="2" max="2" width="29.6719" style="25" customWidth="1"/>
     <col min="3" max="3" width="26.8516" style="25" customWidth="1"/>
-    <col min="4" max="4" width="34.5" style="25" customWidth="1"/>
+    <col min="4" max="4" width="41.6562" style="25" customWidth="1"/>
     <col min="5" max="5" width="101.5" style="25" customWidth="1"/>
     <col min="6" max="6" width="23.5" style="25" customWidth="1"/>
     <col min="7" max="7" width="65.8516" style="25" customWidth="1"/>

</xml_diff>